<commit_message>
Deleted files : trash.py passage de reduce a map reduce sur focntion combine
</commit_message>
<xml_diff>
--- a/file3.xlsx
+++ b/file3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbookpro/Documents/Pythonproject/ProjetSynthese/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E07A0250-DF68-8B48-913F-C72B6BAB0C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F0CB8F-AF16-B84F-BF15-D2202A832E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{77B0BCA4-3E90-3D49-AAC2-DA6C9566F27C}"/>
+    <workbookView xWindow="5560" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{77B0BCA4-3E90-3D49-AAC2-DA6C9566F27C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,39 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>nom</t>
+    <t>prof1</t>
   </si>
   <si>
-    <t>prenom</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>luc</t>
-  </si>
-  <si>
-    <t>as</t>
-  </si>
-  <si>
-    <t>ea</t>
-  </si>
-  <si>
-    <t>victor</t>
-  </si>
-  <si>
-    <t>maj</t>
-  </si>
-  <si>
-    <t>hector</t>
-  </si>
-  <si>
-    <t>salah</t>
-  </si>
-  <si>
-    <t>&amp;é</t>
+    <t>prof2</t>
   </si>
 </sst>
 </file>
@@ -420,67 +393,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44F57892-7930-3C42-8F5B-C2B893A940C3}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B2">
         <v>5</v>
-      </c>
-      <c r="C4">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deleted files : trash.py creation de parseur
</commit_message>
<xml_diff>
--- a/file3.xlsx
+++ b/file3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbookpro/Documents/Pythonproject/ProjetSynthese/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F0CB8F-AF16-B84F-BF15-D2202A832E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44AC6FDF-6D03-8446-9DA1-7115948FFC2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5560" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{77B0BCA4-3E90-3D49-AAC2-DA6C9566F27C}"/>
   </bookViews>
@@ -38,10 +38,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>prof1</t>
+    <t>a</t>
   </si>
   <si>
-    <t>prof2</t>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -396,7 +396,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>